<commit_message>
Take screenshot on test failure
</commit_message>
<xml_diff>
--- a/src/main/resources/data/contactsData.xlsx
+++ b/src/main/resources/data/contactsData.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bambadia/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bambadia/eclipse-workspace/FreeCRMTest/src/main/resources/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7B4D2048-09DC-E248-A96A-82843EDA63F7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6394AC88-842F-6D4B-B3A0-9A174F0DEFB1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="15940" xr2:uid="{54CEC529-1776-EC45-982D-DBF626B8B569}"/>
   </bookViews>
@@ -50,37 +50,37 @@
     <t xml:space="preserve">Joe </t>
   </si>
   <si>
-    <t>Dupont</t>
-  </si>
-  <si>
     <t>VATO</t>
   </si>
   <si>
-    <t>joe@yopmail.com</t>
-  </si>
-  <si>
     <t>Adil</t>
   </si>
   <si>
-    <t xml:space="preserve">Dupont </t>
-  </si>
-  <si>
     <t>VATI</t>
   </si>
   <si>
-    <t>adil@yopmail.com</t>
-  </si>
-  <si>
     <t>Nabi</t>
   </si>
   <si>
-    <t>Dupuis</t>
-  </si>
-  <si>
     <t>VITA</t>
   </si>
   <si>
-    <t>nabi@yopmail.com</t>
+    <t>Dia</t>
+  </si>
+  <si>
+    <t>Dio</t>
+  </si>
+  <si>
+    <t>Dpo</t>
+  </si>
+  <si>
+    <t>joee@yopmail.com</t>
+  </si>
+  <si>
+    <t>adile@yopmail.com</t>
+  </si>
+  <si>
+    <t>nabil@yopmail.com</t>
   </si>
 </sst>
 </file>
@@ -461,7 +461,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -485,38 +485,38 @@
         <v>4</v>
       </c>
       <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" t="s">
-        <v>6</v>
-      </c>
       <c r="D2" s="2" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C3" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" t="s">
         <v>12</v>
       </c>
-      <c r="B4" t="s">
-        <v>13</v>
-      </c>
       <c r="C4" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>15</v>

</xml_diff>